<commit_message>
Added support for multiple sheets of data
</commit_message>
<xml_diff>
--- a/src/downloads/template.xlsx
+++ b/src/downloads/template.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidhochbaum/ae-zoning-api/src/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93834B6-69B6-B043-8887-8728DF09BFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7B06F8-9B29-BF4D-999F-1B8F11738778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2480" yWindow="1640" windowWidth="28040" windowHeight="17440" xr2:uid="{38169481-2C4B-3F4B-8AB3-9A679C630F7E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Template Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="0" sheetId="1" r:id="rId1"/>
+    <sheet name="1" sheetId="4" r:id="rId2"/>
+    <sheet name="2" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,15 +38,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Report Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t xml:space="preserve">Generation Date: </t>
   </si>
   <si>
     <t>Filters:</t>
+  </si>
+  <si>
+    <t>Table:</t>
+  </si>
+  <si>
+    <t>&lt;Report Name&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Date&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Table Name&gt;</t>
   </si>
 </sst>
 </file>
@@ -85,8 +96,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -125,6 +136,116 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{121A206C-18D2-B257-E824-DD61903B4BF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="152400" y="152400"/>
+          <a:ext cx="1562100" cy="752722"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1460500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>92322</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F49EF98-8738-9941-AD82-705D4876584D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="152400" y="152400"/>
+          <a:ext cx="1562100" cy="752722"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1460500</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>92322</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5189BDB-FD2E-0D46-A3C6-7E8964CF9D56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -476,9 +597,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6329681B-5A16-094D-A49B-72A99F0DEB32}">
-  <dimension ref="A6:C10"/>
+  <dimension ref="A6:C17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -489,37 +612,186 @@
   <sheetData>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C8" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A10:C10"/>
     <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56FC30D7-7010-5B47-AEBD-B4627DB6A8F7}">
+  <dimension ref="A6:C17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="3.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A13:C13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B4DE30-A47A-574E-8C5A-A6D905C0BEBB}">
+  <dimension ref="A6:C17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="3.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A13:C13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>